<commit_message>
Corrected variable names and figures
</commit_message>
<xml_diff>
--- a/data/ieh ssg and sit data.xlsx
+++ b/data/ieh ssg and sit data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ea888fd31f257dae/XUSP/GECIFEX/Producoes/Artigos/artigo 1 mestrado - agudo sessao/data analysis – ieh – ssg and sit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ea888fd31f257dae/XUSP/GECIFEX/Producoes/Artigos/artigo 1 mestrado - agudo sessao/data analysis – ieh – ssg and sit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{8040FC65-2FB8-A740-843B-E219EA1277F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{248AB9D2-5B91-9041-A1B9-BCB605AEB206}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="13_ncr:1_{8040FC65-2FB8-A740-843B-E219EA1277F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{741A2BF4-DDD4-6D42-9CB5-8018585FF4E2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{F18DB70B-DB86-7748-975C-1A22E921DACC}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="25600" windowHeight="14180" xr2:uid="{F18DB70B-DB86-7748-975C-1A22E921DACC}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -507,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0FFB8B0-E336-6346-A271-A7366FEC9861}">
   <dimension ref="A1:X35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -519,6 +519,7 @@
     <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="15.6640625" customWidth="1"/>
+    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="34" x14ac:dyDescent="0.2">

</xml_diff>